<commit_message>
create staging table for DF3
</commit_message>
<xml_diff>
--- a/dist/rd3_portal_release.xlsx
+++ b/dist/rd3_portal_release.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>rd3_portal</t>
   </si>
@@ -27,25 +27,22 @@
     <t>RD3 Portal Data</t>
   </si>
   <si>
-    <t>Freezes</t>
+    <t>Releases</t>
   </si>
   <si>
     <t>RD3 portal, containing data submitted by CNAG (v1.1.0, 2021-10-11)</t>
   </si>
   <si>
-    <t>Intermediate tables for RD3 releases (v1.1.0, 2022-01-31)</t>
-  </si>
-  <si>
-    <t>novelwgs</t>
-  </si>
-  <si>
-    <t>Novel WGS</t>
-  </si>
-  <si>
-    <t>Staging table for Novel WGS data (2022-01-31)</t>
-  </si>
-  <si>
-    <t>rd3_portal_release_novelwgs</t>
+    <t>Intermediate tables for RD3 releases</t>
+  </si>
+  <si>
+    <t>rd3_portal_release_freeze3</t>
+  </si>
+  <si>
+    <t>Freeze 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Staging table for Freeze 3 (2022-03-09)</t>
   </si>
   <si>
     <t>id</t>
@@ -580,16 +577,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -632,16 +629,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -673,45 +670,45 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -725,16 +722,16 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -748,16 +745,16 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -771,16 +768,16 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -794,16 +791,16 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -817,16 +814,16 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -840,16 +837,16 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -861,21 +858,21 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -889,16 +886,16 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -912,16 +909,16 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -935,16 +932,16 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -958,16 +955,16 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -981,16 +978,16 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1004,16 +1001,16 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1027,16 +1024,16 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1050,16 +1047,16 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -1073,16 +1070,16 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1096,16 +1093,16 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -1119,16 +1116,16 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1142,16 +1139,16 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1165,16 +1162,16 @@
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1188,16 +1185,16 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1211,16 +1208,16 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1234,16 +1231,16 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>

</xml_diff>